<commit_message>
initial class file added
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gitstuff\TMS\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F3EBED1-13B1-44E5-8C9B-E60C201714F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E310EA7E-1940-46DB-BB23-C4B3744D3A46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="565" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5022" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5686" uniqueCount="343">
   <si>
     <t>testname</t>
   </si>
@@ -873,6 +873,183 @@
   </si>
   <si>
     <t>61</t>
+  </si>
+  <si>
+    <t>AddnewManagerRecordTest</t>
+  </si>
+  <si>
+    <t>Verify that AddnewManagersRecordTest working or not</t>
+  </si>
+  <si>
+    <t>EditManagerRecordTest</t>
+  </si>
+  <si>
+    <t>Verify that EditManagersRecordTest working or not</t>
+  </si>
+  <si>
+    <t>62</t>
+  </si>
+  <si>
+    <t>63</t>
+  </si>
+  <si>
+    <t>AddnewRecordTest</t>
+  </si>
+  <si>
+    <t>Verify that AddnewRecordTest working or not</t>
+  </si>
+  <si>
+    <t>EditRecordTest</t>
+  </si>
+  <si>
+    <t>Verify that EditRecordTest working or not</t>
+  </si>
+  <si>
+    <t>AddnewTrainerRecordTest</t>
+  </si>
+  <si>
+    <t>Verify that AddnewTrainerRecordTest working or not</t>
+  </si>
+  <si>
+    <t>EditTrainerRecordTest</t>
+  </si>
+  <si>
+    <t>Verify that EditTrainerRecordTest working or not</t>
+  </si>
+  <si>
+    <t>64</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>66</t>
+  </si>
+  <si>
+    <t>67</t>
+  </si>
+  <si>
+    <t>Autmation manager</t>
+  </si>
+  <si>
+    <t>automationmanager11@mailinator.com</t>
+  </si>
+  <si>
+    <t>2525421252</t>
+  </si>
+  <si>
+    <t>ie</t>
+  </si>
+  <si>
+    <t>EditManagersRecord</t>
+  </si>
+  <si>
+    <t>9853322523</t>
+  </si>
+  <si>
+    <t>edge</t>
+  </si>
+  <si>
+    <t>Automation Tester</t>
+  </si>
+  <si>
+    <t>automation25@mailinator.com</t>
+  </si>
+  <si>
+    <t>1234567890</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          </t>
+  </si>
+  <si>
+    <t>testing@test.com</t>
+  </si>
+  <si>
+    <t>9858545252</t>
+  </si>
+  <si>
+    <t>Recordaddtesting123</t>
+  </si>
+  <si>
+    <t>recordtesting1223@mailinator.com</t>
+  </si>
+  <si>
+    <t>888121252</t>
+  </si>
+  <si>
+    <t>Trainer testing Experience</t>
+  </si>
+  <si>
+    <t>Linkedin learning courses</t>
+  </si>
+  <si>
+    <t>Details of the trainer regarding courses</t>
+  </si>
+  <si>
+    <t>trainer are located in mailinator</t>
+  </si>
+  <si>
+    <t>Editrecordtesting</t>
+  </si>
+  <si>
+    <t>editrecord12@mailinator.com</t>
+  </si>
+  <si>
+    <t>9876543210</t>
+  </si>
+  <si>
+    <t>testing</t>
+  </si>
+  <si>
+    <t>testing testing</t>
+  </si>
+  <si>
+    <t>test.com</t>
+  </si>
+  <si>
+    <t>firefox</t>
+  </si>
+  <si>
+    <t>AddnewVenueRecordTest</t>
+  </si>
+  <si>
+    <t>Verify that AddnewVenueRecordTest working or not</t>
+  </si>
+  <si>
+    <t>EditVenueRecordTest</t>
+  </si>
+  <si>
+    <t>Verify that EditVenueRecordTest working or not</t>
+  </si>
+  <si>
+    <t>68</t>
+  </si>
+  <si>
+    <t>69</t>
+  </si>
+  <si>
+    <t>AugustTesting</t>
+  </si>
+  <si>
+    <t>August Floor</t>
+  </si>
+  <si>
+    <t>August Unit</t>
+  </si>
+  <si>
+    <t>AugustBuliding</t>
+  </si>
+  <si>
+    <t>August Room</t>
+  </si>
+  <si>
+    <t>654321</t>
+  </si>
+  <si>
+    <t>Edit Automation</t>
+  </si>
+  <si>
+    <t>987654</t>
   </si>
 </sst>
 </file>
@@ -1204,10 +1381,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E62"/>
+  <dimension ref="A1:E70"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -2264,12 +2441,148 @@
         <v>169</v>
       </c>
       <c r="C62" t="s">
-        <v>7</v>
+        <v>195</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>283</v>
       </c>
       <c r="E62" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" t="s">
+        <v>284</v>
+      </c>
+      <c r="B63" t="s">
+        <v>285</v>
+      </c>
+      <c r="C63" t="s">
+        <v>195</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" t="s">
+        <v>286</v>
+      </c>
+      <c r="B64" t="s">
+        <v>287</v>
+      </c>
+      <c r="C64" t="s">
+        <v>195</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" t="s">
+        <v>290</v>
+      </c>
+      <c r="B65" t="s">
+        <v>291</v>
+      </c>
+      <c r="C65" t="s">
+        <v>195</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" t="s">
+        <v>292</v>
+      </c>
+      <c r="B66" t="s">
+        <v>293</v>
+      </c>
+      <c r="C66" t="s">
+        <v>195</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" t="s">
+        <v>294</v>
+      </c>
+      <c r="B67" t="s">
+        <v>295</v>
+      </c>
+      <c r="C67" t="s">
+        <v>195</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" t="s">
+        <v>296</v>
+      </c>
+      <c r="B68" t="s">
+        <v>297</v>
+      </c>
+      <c r="C68" t="s">
+        <v>195</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" t="s">
+        <v>329</v>
+      </c>
+      <c r="B69" t="s">
+        <v>330</v>
+      </c>
+      <c r="C69" t="s">
+        <v>7</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" t="s">
+        <v>331</v>
+      </c>
+      <c r="B70" t="s">
+        <v>332</v>
+      </c>
+      <c r="C70" t="s">
+        <v>195</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="E70" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2281,10 +2594,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:BJ76"/>
+  <dimension ref="A1:EP86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A85" sqref="A85"/>
     </sheetView>
   </sheetViews>
@@ -14345,7 +14658,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="65" spans="1:62">
+    <row r="65" spans="1:146">
       <c r="A65" s="3" t="s">
         <v>224</v>
       </c>
@@ -14533,7 +14846,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="66" spans="1:62">
+    <row r="66" spans="1:146">
       <c r="A66" s="3" t="s">
         <v>225</v>
       </c>
@@ -14721,7 +15034,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="67" spans="1:62">
+    <row r="67" spans="1:146">
       <c r="A67" s="3" t="s">
         <v>226</v>
       </c>
@@ -14909,7 +15222,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="68" spans="1:62">
+    <row r="68" spans="1:146">
       <c r="A68" s="3" t="s">
         <v>227</v>
       </c>
@@ -15097,7 +15410,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="69" spans="1:62">
+    <row r="69" spans="1:146">
       <c r="A69" t="s">
         <v>232</v>
       </c>
@@ -15285,7 +15598,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="70" spans="1:62">
+    <row r="70" spans="1:146">
       <c r="A70" t="s">
         <v>234</v>
       </c>
@@ -15473,7 +15786,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="71" spans="1:62">
+    <row r="71" spans="1:146">
       <c r="A71" t="s">
         <v>242</v>
       </c>
@@ -15661,7 +15974,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="72" spans="1:62">
+    <row r="72" spans="1:146">
       <c r="A72" t="s">
         <v>265</v>
       </c>
@@ -15849,7 +16162,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="73" spans="1:62">
+    <row r="73" spans="1:146">
       <c r="A73" t="s">
         <v>271</v>
       </c>
@@ -16037,7 +16350,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="74" spans="1:62">
+    <row r="74" spans="1:146">
       <c r="A74" t="s">
         <v>273</v>
       </c>
@@ -16225,7 +16538,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="75" spans="1:62">
+    <row r="75" spans="1:146">
       <c r="A75" t="s">
         <v>280</v>
       </c>
@@ -16413,12 +16726,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="76" spans="1:62">
+    <row r="76" spans="1:146">
       <c r="A76" t="s">
         <v>282</v>
       </c>
       <c r="B76" t="s">
-        <v>7</v>
+        <v>195</v>
       </c>
       <c r="C76" t="s">
         <v>81</v>
@@ -16601,7 +16914,1904 @@
         <v>84</v>
       </c>
     </row>
+    <row r="77" spans="1:146">
+      <c r="A77" t="s">
+        <v>284</v>
+      </c>
+      <c r="B77" t="s">
+        <v>195</v>
+      </c>
+      <c r="C77" t="s">
+        <v>81</v>
+      </c>
+      <c r="D77" t="s">
+        <v>82</v>
+      </c>
+      <c r="E77" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F77" t="s">
+        <v>126</v>
+      </c>
+      <c r="G77" t="s">
+        <v>135</v>
+      </c>
+      <c r="H77" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="I77" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="J77" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K77" t="s">
+        <v>302</v>
+      </c>
+      <c r="L77" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="M77" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="N77" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="O77" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="P77" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q77" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="R77" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="S77" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="T77" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="U77" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="V77" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="W77" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="X77" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y77" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="Z77" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AA77" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AB77" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC77" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD77" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE77" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AF77" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AG77" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AH77" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AI77" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AJ77" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK77" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AL77" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AM77" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AN77" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AO77" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AP77" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AQ77" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AR77" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AS77" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AT77" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AU77" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AV77" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AW77" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AX77" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AY77" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AZ77" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BA77" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BB77" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BC77" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BD77" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BE77" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BF77" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BG77" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BH77" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BI77" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BJ77" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="EP77" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="78" spans="1:146">
+      <c r="A78" t="s">
+        <v>286</v>
+      </c>
+      <c r="B78" t="s">
+        <v>195</v>
+      </c>
+      <c r="C78" t="s">
+        <v>81</v>
+      </c>
+      <c r="D78" t="s">
+        <v>82</v>
+      </c>
+      <c r="E78" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F78" t="s">
+        <v>126</v>
+      </c>
+      <c r="G78" t="s">
+        <v>135</v>
+      </c>
+      <c r="H78" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="I78" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="J78" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K78" t="s">
+        <v>306</v>
+      </c>
+      <c r="L78" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="M78" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="N78" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="O78" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="P78" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q78" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="R78" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="S78" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="T78" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="U78" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="V78" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="W78" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="X78" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y78" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="Z78" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AA78" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AB78" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC78" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD78" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE78" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AF78" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AG78" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AH78" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AI78" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AJ78" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK78" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AL78" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AM78" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AN78" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AO78" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AP78" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AQ78" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AR78" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AS78" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AT78" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AU78" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AV78" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AW78" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AX78" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AY78" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AZ78" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BA78" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BB78" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BC78" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BD78" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BE78" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BF78" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BG78" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BH78" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BI78" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BJ78" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="EP78" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="79" spans="1:146">
+      <c r="A79" t="s">
+        <v>290</v>
+      </c>
+      <c r="B79" t="s">
+        <v>195</v>
+      </c>
+      <c r="C79" t="s">
+        <v>81</v>
+      </c>
+      <c r="D79" t="s">
+        <v>82</v>
+      </c>
+      <c r="E79" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F79" t="s">
+        <v>126</v>
+      </c>
+      <c r="G79" t="s">
+        <v>128</v>
+      </c>
+      <c r="H79" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="I79" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="J79" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K79" t="s">
+        <v>309</v>
+      </c>
+      <c r="L79" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="M79" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="N79" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="O79" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="P79" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q79" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="R79" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="S79" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="T79" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="U79" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="V79" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="W79" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="X79" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y79" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="Z79" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AA79" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AB79" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC79" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD79" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE79" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AF79" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AG79" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AH79" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AI79" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AJ79" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK79" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AL79" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AM79" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AN79" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AO79" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AP79" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AQ79" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AR79" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AS79" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AT79" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AU79" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AV79" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AW79" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AX79" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AY79" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AZ79" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BA79" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BB79" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BC79" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BD79" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BE79" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BF79" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BG79" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BH79" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BI79" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BJ79" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="80" spans="1:146">
+      <c r="A80" t="s">
+        <v>290</v>
+      </c>
+      <c r="B80" t="s">
+        <v>195</v>
+      </c>
+      <c r="C80" t="s">
+        <v>81</v>
+      </c>
+      <c r="D80" t="s">
+        <v>82</v>
+      </c>
+      <c r="E80" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F80" t="s">
+        <v>126</v>
+      </c>
+      <c r="G80" t="s">
+        <v>128</v>
+      </c>
+      <c r="H80" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="I80" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="J80" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K80" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="L80" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="M80" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="N80" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="O80" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="P80" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q80" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="R80" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="S80" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="T80" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="U80" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="V80" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="W80" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="X80" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y80" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="Z80" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AA80" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AB80" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC80" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD80" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE80" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AF80" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AG80" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AH80" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AI80" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AJ80" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK80" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AL80" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AM80" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AN80" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AO80" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AP80" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AQ80" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AR80" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AS80" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AT80" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AU80" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AV80" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AW80" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AX80" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AY80" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AZ80" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BA80" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BB80" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BC80" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BD80" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BE80" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BF80" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BG80" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BH80" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BI80" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BJ80" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="81" spans="1:146">
+      <c r="A81" t="s">
+        <v>290</v>
+      </c>
+      <c r="B81" t="s">
+        <v>195</v>
+      </c>
+      <c r="C81" t="s">
+        <v>81</v>
+      </c>
+      <c r="D81" t="s">
+        <v>82</v>
+      </c>
+      <c r="E81" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F81" t="s">
+        <v>126</v>
+      </c>
+      <c r="G81" t="s">
+        <v>128</v>
+      </c>
+      <c r="H81" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="I81" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="J81" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K81" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="L81" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="M81" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="N81" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="O81" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="P81" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q81" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="R81" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="S81" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="T81" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="U81" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="V81" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="W81" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="X81" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y81" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="Z81" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AA81" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AB81" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC81" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD81" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE81" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AF81" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AG81" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AH81" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AI81" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AJ81" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK81" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AL81" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AM81" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AN81" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AO81" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AP81" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AQ81" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AR81" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AS81" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AT81" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AU81" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AV81" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AW81" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AX81" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AY81" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AZ81" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BA81" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BB81" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BC81" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BD81" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BE81" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BF81" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BG81" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BH81" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BI81" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BJ81" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="82" spans="1:146">
+      <c r="A82" t="s">
+        <v>292</v>
+      </c>
+      <c r="B82" t="s">
+        <v>195</v>
+      </c>
+      <c r="C82" t="s">
+        <v>81</v>
+      </c>
+      <c r="D82" t="s">
+        <v>82</v>
+      </c>
+      <c r="E82" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F82" t="s">
+        <v>126</v>
+      </c>
+      <c r="G82" t="s">
+        <v>128</v>
+      </c>
+      <c r="H82" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="I82" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="J82" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K82" t="s">
+        <v>241</v>
+      </c>
+      <c r="L82" t="s">
+        <v>313</v>
+      </c>
+      <c r="M82" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="N82" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="O82" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="P82" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q82" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="R82" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="S82" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="T82" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="U82" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="V82" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="W82" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="X82" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y82" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="Z82" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AA82" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AB82" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC82" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD82" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE82" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AF82" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AG82" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AH82" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AI82" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AJ82" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK82" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AL82" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AM82" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AN82" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AO82" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AP82" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AQ82" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AR82" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AS82" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AT82" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AU82" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AV82" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AW82" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AX82" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AY82" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AZ82" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BA82" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BB82" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BC82" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BD82" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BE82" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BF82" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BG82" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BH82" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BI82" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BJ82" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="83" spans="1:146">
+      <c r="A83" t="s">
+        <v>294</v>
+      </c>
+      <c r="B83" t="s">
+        <v>195</v>
+      </c>
+      <c r="C83" t="s">
+        <v>81</v>
+      </c>
+      <c r="D83" t="s">
+        <v>82</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F83" t="s">
+        <v>126</v>
+      </c>
+      <c r="G83" t="s">
+        <v>127</v>
+      </c>
+      <c r="H83" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="I83" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="J83" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K83" t="s">
+        <v>315</v>
+      </c>
+      <c r="L83" t="s">
+        <v>316</v>
+      </c>
+      <c r="M83" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="N83" t="s">
+        <v>318</v>
+      </c>
+      <c r="O83" t="s">
+        <v>319</v>
+      </c>
+      <c r="P83" t="s">
+        <v>320</v>
+      </c>
+      <c r="Q83" t="s">
+        <v>321</v>
+      </c>
+      <c r="R83" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="S83" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="T83" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="U83" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="V83" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="W83" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="X83" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y83" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="Z83" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AA83" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AB83" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC83" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD83" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE83" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AF83" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AG83" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AH83" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AI83" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AJ83" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK83" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AL83" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AM83" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AN83" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AO83" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AP83" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AQ83" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AR83" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AS83" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AT83" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AU83" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AV83" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AW83" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AX83" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AY83" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AZ83" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BA83" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BB83" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BC83" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BD83" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BE83" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BF83" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BG83" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BH83" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BI83" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BJ83" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="EP83" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="84" spans="1:146">
+      <c r="A84" t="s">
+        <v>296</v>
+      </c>
+      <c r="B84" t="s">
+        <v>195</v>
+      </c>
+      <c r="C84" t="s">
+        <v>81</v>
+      </c>
+      <c r="D84" t="s">
+        <v>82</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F84" t="s">
+        <v>126</v>
+      </c>
+      <c r="G84" t="s">
+        <v>127</v>
+      </c>
+      <c r="H84" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="I84" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="J84" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K84" t="s">
+        <v>322</v>
+      </c>
+      <c r="L84" t="s">
+        <v>323</v>
+      </c>
+      <c r="M84" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="N84" t="s">
+        <v>325</v>
+      </c>
+      <c r="O84" t="s">
+        <v>326</v>
+      </c>
+      <c r="P84" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q84" t="s">
+        <v>327</v>
+      </c>
+      <c r="R84" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="S84" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="T84" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="U84" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="V84" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="W84" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="X84" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y84" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="Z84" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AA84" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AB84" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC84" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD84" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE84" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AF84" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AG84" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AH84" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AI84" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AJ84" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK84" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AL84" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AM84" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AN84" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AO84" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AP84" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AQ84" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AR84" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AS84" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AT84" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AU84" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AV84" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AW84" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AX84" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AY84" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AZ84" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BA84" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BB84" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BC84" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BD84" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BE84" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BF84" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BG84" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BH84" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BI84" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BJ84" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="EP84" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="85" spans="1:146">
+      <c r="A85" t="s">
+        <v>329</v>
+      </c>
+      <c r="B85" t="s">
+        <v>7</v>
+      </c>
+      <c r="C85" t="s">
+        <v>81</v>
+      </c>
+      <c r="D85" t="s">
+        <v>82</v>
+      </c>
+      <c r="E85" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F85" t="s">
+        <v>125</v>
+      </c>
+      <c r="G85" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="H85" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="I85" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="J85" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K85" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="L85" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="M85" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="N85" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="O85" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="P85" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q85" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="R85" t="s">
+        <v>335</v>
+      </c>
+      <c r="S85" t="s">
+        <v>335</v>
+      </c>
+      <c r="T85" t="s">
+        <v>336</v>
+      </c>
+      <c r="U85" t="s">
+        <v>337</v>
+      </c>
+      <c r="V85" t="s">
+        <v>338</v>
+      </c>
+      <c r="W85" t="s">
+        <v>339</v>
+      </c>
+      <c r="X85" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="Y85" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="Z85" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AA85" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AB85" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC85" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD85" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE85" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AF85" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AG85" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AH85" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AI85" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AJ85" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK85" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AL85" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AM85" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AN85" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AO85" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AP85" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AQ85" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AR85" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AS85" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AT85" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AU85" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AV85" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AW85" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AX85" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AY85" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AZ85" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BA85" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BB85" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BC85" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BD85" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BE85" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BF85" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BG85" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BH85" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BI85" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BJ85" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" spans="1:146">
+      <c r="A86" t="s">
+        <v>331</v>
+      </c>
+      <c r="B86" t="s">
+        <v>195</v>
+      </c>
+      <c r="C86" t="s">
+        <v>81</v>
+      </c>
+      <c r="D86" t="s">
+        <v>82</v>
+      </c>
+      <c r="E86" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F86" t="s">
+        <v>125</v>
+      </c>
+      <c r="G86" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="H86" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="I86" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="J86" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K86" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="L86" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="M86" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="N86" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="O86" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="P86" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q86" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="R86" t="s">
+        <v>341</v>
+      </c>
+      <c r="S86" t="s">
+        <v>341</v>
+      </c>
+      <c r="T86" t="s">
+        <v>341</v>
+      </c>
+      <c r="U86" t="s">
+        <v>341</v>
+      </c>
+      <c r="V86" t="s">
+        <v>341</v>
+      </c>
+      <c r="W86" t="s">
+        <v>341</v>
+      </c>
+      <c r="X86" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="Y86" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="Z86" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AA86" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AB86" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC86" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD86" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE86" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AF86" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AG86" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AH86" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AI86" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AJ86" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK86" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AL86" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AM86" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AN86" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AO86" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AP86" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AQ86" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AR86" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AS86" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AT86" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AU86" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AV86" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AW86" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AX86" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AY86" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AZ86" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BA86" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BB86" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BC86" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BD86" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BE86" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BF86" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BG86" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BH86" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BI86" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BJ86" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="EP77:EP78 EP83:EP84" xr:uid="{0B9943E6-E268-434F-9E4C-123BB136FD63}">
+      <formula1>$EP$45:$EP$48</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add new testcase in courserun
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gitstuff\TMS\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92D7AD03-02BA-4CA3-8DA4-4ABE8CACA384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9EF15D9-15A5-4E91-9D24-636BD53291A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="565" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5753" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6088" uniqueCount="361">
   <si>
     <t>testname</t>
   </si>
@@ -1059,6 +1059,51 @@
   </si>
   <si>
     <t>70</t>
+  </si>
+  <si>
+    <t>AccessTraineeListTab</t>
+  </si>
+  <si>
+    <t>Verify user is able to access trainee list tab</t>
+  </si>
+  <si>
+    <t>71</t>
+  </si>
+  <si>
+    <t>AccessSoftBookingsTab</t>
+  </si>
+  <si>
+    <t>AccessWaitingListTab</t>
+  </si>
+  <si>
+    <t>AccessPaymentsListTab</t>
+  </si>
+  <si>
+    <t>AccessRefershersTab</t>
+  </si>
+  <si>
+    <t>Verify user is able to access SoftBookingsTab</t>
+  </si>
+  <si>
+    <t>Verify user is able to access WaitingListTab</t>
+  </si>
+  <si>
+    <t>Verify user is able to access PaymentsListTab</t>
+  </si>
+  <si>
+    <t>Verify user is able to access RefershersTab</t>
+  </si>
+  <si>
+    <t>72</t>
+  </si>
+  <si>
+    <t>73</t>
+  </si>
+  <si>
+    <t>74</t>
+  </si>
+  <si>
+    <t>75</t>
   </si>
 </sst>
 </file>
@@ -1390,10 +1435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E71"/>
+  <dimension ref="A1:E76"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68:C70"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="A72" sqref="A72:A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -2603,12 +2648,97 @@
         <v>344</v>
       </c>
       <c r="C71" t="s">
-        <v>7</v>
+        <v>195</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>345</v>
       </c>
       <c r="E71" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" t="s">
+        <v>346</v>
+      </c>
+      <c r="B72" t="s">
+        <v>347</v>
+      </c>
+      <c r="C72" t="s">
+        <v>7</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" t="s">
+        <v>349</v>
+      </c>
+      <c r="B73" t="s">
+        <v>353</v>
+      </c>
+      <c r="C73" t="s">
+        <v>7</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" t="s">
+        <v>350</v>
+      </c>
+      <c r="B74" t="s">
+        <v>354</v>
+      </c>
+      <c r="C74" t="s">
+        <v>7</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" t="s">
+        <v>351</v>
+      </c>
+      <c r="B75" t="s">
+        <v>355</v>
+      </c>
+      <c r="C75" t="s">
+        <v>7</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" t="s">
+        <v>352</v>
+      </c>
+      <c r="B76" t="s">
+        <v>356</v>
+      </c>
+      <c r="C76" t="s">
+        <v>7</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="E76" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2620,11 +2750,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:EI87"/>
+  <dimension ref="A1:EI92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A87" sqref="A87"/>
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E85" sqref="E85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -18837,7 +18967,7 @@
         <v>343</v>
       </c>
       <c r="B87" t="s">
-        <v>7</v>
+        <v>195</v>
       </c>
       <c r="C87" t="s">
         <v>81</v>
@@ -19017,6 +19147,946 @@
         <v>84</v>
       </c>
       <c r="BJ87" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="88" spans="1:139">
+      <c r="A88" t="s">
+        <v>346</v>
+      </c>
+      <c r="B88" t="s">
+        <v>7</v>
+      </c>
+      <c r="C88" t="s">
+        <v>81</v>
+      </c>
+      <c r="D88" t="s">
+        <v>82</v>
+      </c>
+      <c r="E88" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F88" t="s">
+        <v>133</v>
+      </c>
+      <c r="G88" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="H88" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="I88" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="J88" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K88" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="L88" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="M88" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="N88" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="O88" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="P88" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q88" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="R88" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="S88" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="T88" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="U88" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="V88" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="W88" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="X88" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y88" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="Z88" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AA88" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AB88" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC88" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD88" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE88" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AF88" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AG88" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AH88" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AI88" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AJ88" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK88" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AL88" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AM88" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AN88" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AO88" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AP88" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AQ88" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AR88" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AS88" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AT88" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AU88" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AV88" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AW88" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AX88" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AY88" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AZ88" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BA88" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BB88" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BC88" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BD88" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BE88" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BF88" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BG88" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BH88" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BI88" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BJ88" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="89" spans="1:139">
+      <c r="A89" t="s">
+        <v>349</v>
+      </c>
+      <c r="B89" t="s">
+        <v>7</v>
+      </c>
+      <c r="C89" t="s">
+        <v>81</v>
+      </c>
+      <c r="D89" t="s">
+        <v>82</v>
+      </c>
+      <c r="E89" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F89" t="s">
+        <v>133</v>
+      </c>
+      <c r="G89" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="H89" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="I89" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="J89" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K89" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="L89" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="M89" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="N89" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="O89" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="P89" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q89" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="R89" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="S89" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="T89" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="U89" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="V89" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="W89" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="X89" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y89" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="Z89" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AA89" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AB89" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC89" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD89" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE89" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AF89" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AG89" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AH89" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AI89" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AJ89" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK89" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AL89" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AM89" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AN89" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AO89" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AP89" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AQ89" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AR89" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AS89" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AT89" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AU89" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AV89" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AW89" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AX89" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AY89" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AZ89" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BA89" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BB89" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BC89" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BD89" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BE89" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BF89" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BG89" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BH89" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BI89" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BJ89" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="90" spans="1:139">
+      <c r="A90" t="s">
+        <v>350</v>
+      </c>
+      <c r="B90" t="s">
+        <v>7</v>
+      </c>
+      <c r="C90" t="s">
+        <v>81</v>
+      </c>
+      <c r="D90" t="s">
+        <v>82</v>
+      </c>
+      <c r="E90" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F90" t="s">
+        <v>133</v>
+      </c>
+      <c r="G90" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="H90" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="I90" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="J90" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K90" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="L90" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="M90" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="N90" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="O90" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="P90" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q90" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="R90" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="S90" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="T90" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="U90" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="V90" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="W90" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="X90" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y90" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="Z90" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AA90" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AB90" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC90" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD90" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE90" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AF90" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AG90" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AH90" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AI90" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AJ90" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK90" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AL90" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AM90" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AN90" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AO90" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AP90" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AQ90" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AR90" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AS90" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AT90" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AU90" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AV90" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AW90" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AX90" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AY90" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AZ90" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BA90" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BB90" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BC90" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BD90" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BE90" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BF90" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BG90" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BH90" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BI90" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BJ90" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="91" spans="1:139">
+      <c r="A91" t="s">
+        <v>351</v>
+      </c>
+      <c r="B91" t="s">
+        <v>7</v>
+      </c>
+      <c r="C91" t="s">
+        <v>81</v>
+      </c>
+      <c r="D91" t="s">
+        <v>82</v>
+      </c>
+      <c r="E91" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F91" t="s">
+        <v>133</v>
+      </c>
+      <c r="G91" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="H91" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="I91" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="J91" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K91" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="L91" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="M91" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="N91" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="O91" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="P91" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q91" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="R91" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="S91" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="T91" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="U91" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="V91" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="W91" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="X91" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y91" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="Z91" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AA91" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AB91" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC91" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD91" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE91" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AF91" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AG91" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AH91" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AI91" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AJ91" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK91" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AL91" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AM91" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AN91" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AO91" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AP91" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AQ91" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AR91" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AS91" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AT91" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AU91" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AV91" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AW91" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AX91" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AY91" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AZ91" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BA91" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BB91" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BC91" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BD91" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BE91" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BF91" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BG91" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BH91" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BI91" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BJ91" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="92" spans="1:139">
+      <c r="A92" t="s">
+        <v>352</v>
+      </c>
+      <c r="B92" t="s">
+        <v>7</v>
+      </c>
+      <c r="C92" t="s">
+        <v>81</v>
+      </c>
+      <c r="D92" t="s">
+        <v>82</v>
+      </c>
+      <c r="E92" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F92" t="s">
+        <v>133</v>
+      </c>
+      <c r="G92" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="H92" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="I92" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="J92" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K92" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="L92" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="M92" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="N92" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="O92" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="P92" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q92" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="R92" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="S92" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="T92" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="U92" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="V92" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="W92" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="X92" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y92" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="Z92" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AA92" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AB92" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC92" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD92" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE92" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AF92" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AG92" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AH92" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AI92" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AJ92" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK92" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AL92" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AM92" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AN92" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AO92" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AP92" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AQ92" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AR92" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AS92" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AT92" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AU92" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AV92" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AW92" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AX92" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AY92" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AZ92" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BA92" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BB92" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BC92" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BD92" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BE92" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BF92" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BG92" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BH92" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BI92" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BJ92" s="3" t="s">
         <v>84</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Student enrollment test added
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gitstuff\TMS\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9EF15D9-15A5-4E91-9D24-636BD53291A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B021B6D-43AC-4F61-AA66-E8F0096A0579}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="565" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6088" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6155" uniqueCount="379">
   <si>
     <t>testname</t>
   </si>
@@ -1104,6 +1104,60 @@
   </si>
   <si>
     <t>75</t>
+  </si>
+  <si>
+    <t>AddStudentEnrollmentRecordTest</t>
+  </si>
+  <si>
+    <t>Verify that user is able to add student enrollment record in TMS application</t>
+  </si>
+  <si>
+    <t>76</t>
+  </si>
+  <si>
+    <t>Digital Marketing 1</t>
+  </si>
+  <si>
+    <t>Ronald Christian</t>
+  </si>
+  <si>
+    <t>S3010700D</t>
+  </si>
+  <si>
+    <t>65253625</t>
+  </si>
+  <si>
+    <t>ronald@mailinator.com</t>
+  </si>
+  <si>
+    <t>10/10/1998</t>
+  </si>
+  <si>
+    <t>2Stallions</t>
+  </si>
+  <si>
+    <t>Roma Edward</t>
+  </si>
+  <si>
+    <t>romaedward@mailinator.com</t>
+  </si>
+  <si>
+    <t>85956525</t>
+  </si>
+  <si>
+    <t>edward@mailinator.com</t>
+  </si>
+  <si>
+    <t>256521</t>
+  </si>
+  <si>
+    <t>Testing Student Enrollment</t>
+  </si>
+  <si>
+    <t>799</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -1435,10 +1489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E76"/>
+  <dimension ref="A1:E77"/>
   <sheetViews>
     <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72:A76"/>
+      <selection activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -2665,7 +2719,7 @@
         <v>347</v>
       </c>
       <c r="C72" t="s">
-        <v>7</v>
+        <v>195</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>348</v>
@@ -2682,7 +2736,7 @@
         <v>353</v>
       </c>
       <c r="C73" t="s">
-        <v>7</v>
+        <v>195</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>357</v>
@@ -2699,7 +2753,7 @@
         <v>354</v>
       </c>
       <c r="C74" t="s">
-        <v>7</v>
+        <v>195</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>358</v>
@@ -2716,7 +2770,7 @@
         <v>355</v>
       </c>
       <c r="C75" t="s">
-        <v>7</v>
+        <v>195</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>359</v>
@@ -2733,12 +2787,29 @@
         <v>356</v>
       </c>
       <c r="C76" t="s">
-        <v>7</v>
+        <v>195</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>360</v>
       </c>
       <c r="E76" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" t="s">
+        <v>361</v>
+      </c>
+      <c r="B77" t="s">
+        <v>362</v>
+      </c>
+      <c r="C77" t="s">
+        <v>7</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="E77" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2750,11 +2821,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:EI92"/>
+  <dimension ref="A1:EI93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E85" sqref="E85"/>
+    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AL93" sqref="AL93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -19155,7 +19226,7 @@
         <v>346</v>
       </c>
       <c r="B88" t="s">
-        <v>7</v>
+        <v>195</v>
       </c>
       <c r="C88" t="s">
         <v>81</v>
@@ -19343,7 +19414,7 @@
         <v>349</v>
       </c>
       <c r="B89" t="s">
-        <v>7</v>
+        <v>195</v>
       </c>
       <c r="C89" t="s">
         <v>81</v>
@@ -19531,7 +19602,7 @@
         <v>350</v>
       </c>
       <c r="B90" t="s">
-        <v>7</v>
+        <v>195</v>
       </c>
       <c r="C90" t="s">
         <v>81</v>
@@ -19719,7 +19790,7 @@
         <v>351</v>
       </c>
       <c r="B91" t="s">
-        <v>7</v>
+        <v>195</v>
       </c>
       <c r="C91" t="s">
         <v>81</v>
@@ -19907,7 +19978,7 @@
         <v>352</v>
       </c>
       <c r="B92" t="s">
-        <v>7</v>
+        <v>195</v>
       </c>
       <c r="C92" t="s">
         <v>81</v>
@@ -20087,6 +20158,194 @@
         <v>84</v>
       </c>
       <c r="BJ92" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="93" spans="1:139">
+      <c r="A93" t="s">
+        <v>361</v>
+      </c>
+      <c r="B93" t="s">
+        <v>7</v>
+      </c>
+      <c r="C93" t="s">
+        <v>81</v>
+      </c>
+      <c r="D93" t="s">
+        <v>82</v>
+      </c>
+      <c r="E93" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F93" t="s">
+        <v>130</v>
+      </c>
+      <c r="G93" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="H93" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="I93" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="J93" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="K93" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="L93" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="M93" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="N93" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="O93" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="P93" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q93" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="R93" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="S93" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="T93" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="U93" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="V93" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="W93" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="X93" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y93" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="Z93" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AA93" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AB93" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC93" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD93" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="AE93" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="AF93" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="AG93" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="AH93" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="AI93" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="AJ93" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK93" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="AL93" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="AM93" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="AN93" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="AO93" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="AP93" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="AQ93" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="AR93" s="3" t="s">
+        <v>377</v>
+      </c>
+      <c r="AS93" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="AT93" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AU93" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AV93" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AW93" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AX93" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AY93" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="AZ93" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="BA93" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BB93" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BC93" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BD93" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BE93" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BF93" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BG93" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BH93" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BI93" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="BJ93" s="3" t="s">
         <v>84</v>
       </c>
     </row>

</xml_diff>